<commit_message>
changed date request (front+back)
</commit_message>
<xml_diff>
--- a/src/main/resources/patterns.xlsx
+++ b/src/main/resources/patterns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Запрос 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>##</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>unhcr_date</t>
-  </si>
-  <si>
-    <t>sd</t>
   </si>
   <si>
     <t>un_relationship_cd</t>
@@ -263,18 +260,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -426,17 +417,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -518,11 +498,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -539,104 +528,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,51 +930,34 @@
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="8">
-        <v>8</v>
-      </c>
-      <c r="J1" s="8">
-        <v>9</v>
-      </c>
-      <c r="K1" s="7">
-        <v>10</v>
-      </c>
-      <c r="L1" s="7">
-        <v>11</v>
-      </c>
-      <c r="M1" s="8">
-        <v>12</v>
-      </c>
-      <c r="N1" s="8">
-        <v>13</v>
-      </c>
-      <c r="O1" s="8">
-        <v>14</v>
-      </c>
-      <c r="P1" s="7">
-        <v>15</v>
-      </c>
+      <c r="I1" s="41"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I2" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="I2" s="42"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
       <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1000,16 +976,16 @@
       <c r="N3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="9" t="s">
-        <v>20</v>
+      <c r="O3" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1022,42 +998,42 @@
       <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="10"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1081,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1097,80 +1073,80 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C2" s="14">
+      <c r="C2" s="12">
         <v>42441</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="14">
+      <c r="C3" s="12">
         <v>42382</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="14"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="O6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="31"/>
-      <c r="O6" s="31" t="s">
+      <c r="P6" s="30"/>
+    </row>
+    <row r="8" spans="2:16" s="15" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="P6" s="31"/>
-    </row>
-    <row r="8" spans="2:16" s="17" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="G8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="H8" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="J8" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22" t="s">
+      <c r="K8" s="19"/>
+      <c r="L8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="23"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="23"/>
+      <c r="B9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="21"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1200,68 +1176,68 @@
   <sheetData>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="15" t="s">
+    </row>
+    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="F5" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="G5" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="27" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="36"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1281,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AC17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1298,247 +1274,247 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="B2" s="12"/>
+      <c r="G2" s="12"/>
       <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="12">
+        <v>42441</v>
+      </c>
+    </row>
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="14">
-        <v>42441</v>
-      </c>
-    </row>
-    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="14">
+      <c r="J3" s="12">
         <v>42382</v>
       </c>
     </row>
     <row r="4" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="2:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38" t="s">
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" spans="2:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-    </row>
-    <row r="6" spans="2:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+    </row>
+    <row r="7" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-    </row>
-    <row r="7" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="39" t="s">
+      <c r="D7" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="E7" s="39"/>
+      <c r="F7" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40" t="s">
+      <c r="G7" s="39"/>
+      <c r="H7" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40" t="s">
+      <c r="I7" s="39"/>
+    </row>
+    <row r="8" spans="2:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="38"/>
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8" spans="2:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="39"/>
-      <c r="D8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="20"/>
-    </row>
-    <row r="11" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="12" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="13" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="19">
+      <c r="D13" s="17">
         <f>D9+D10+D11+D12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="18">
         <f>E9+E10+E1+E12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <f>F9+F10+F1+F12</f>
         <v>0</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="18">
         <f>G9+G10+G1+G12</f>
         <v>0</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="17">
         <f>H9+H10+H1+H12</f>
         <v>0</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="18">
         <f>I9+I10+I1+I12</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="V14" s="31" t="s">
+      <c r="V14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="W14" s="30"/>
+      <c r="AA14" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="W14" s="31"/>
-      <c r="AA14" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB14" s="31"/>
-    </row>
-    <row r="16" spans="2:29" s="17" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K16" s="22" t="s">
+      <c r="AB14" s="30"/>
+    </row>
+    <row r="16" spans="2:29" s="15" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="N16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="Q16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="R16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="S16" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="T16" s="19"/>
+      <c r="U16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="W16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="22" t="s">
+      <c r="X16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="P16" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q16" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="R16" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="S16" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="V16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="W16" s="22" t="s">
+      <c r="AB16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="X16" s="22" t="s">
+      <c r="AC16" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Z16" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC16" s="22" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="17" spans="11:29" x14ac:dyDescent="0.25">
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="21"/>
+      <c r="AC17" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
report one without family members output
</commit_message>
<xml_diff>
--- a/src/main/resources/patterns.xlsx
+++ b/src/main/resources/patterns.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>##</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>total family members</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -576,9 +579,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -586,30 +586,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -635,9 +647,6 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -920,81 +929,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="9" max="14" width="16.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="9" max="15" width="16.5703125" customWidth="1"/>
+    <col min="16" max="16" width="20.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="44"/>
-      <c r="I1" s="25"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="28"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="21"/>
-      <c r="K1" s="5"/>
+      <c r="K1" s="27"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I2" s="26"/>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="M1" s="5"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="25"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="32"/>
       <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="R3" s="22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
+    <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1009,43 +1024,44 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="7"/>
+      <c r="K4" s="27"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="5"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="23"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="P4" s="14"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="29"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1104,14 +1120,14 @@
       <c r="C4" s="11"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="34"/>
-      <c r="O6" s="34" t="s">
+      <c r="M6" s="37"/>
+      <c r="O6" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="34"/>
+      <c r="P6" s="37"/>
     </row>
     <row r="8" spans="2:16" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -1214,40 +1230,40 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
@@ -1317,48 +1333,48 @@
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="2:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="40" t="s">
+      <c r="C5" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41" t="s">
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="2:29" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
     </row>
     <row r="7" spans="2:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
+      <c r="E7" s="46"/>
+      <c r="F7" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43" t="s">
+      <c r="G7" s="46"/>
+      <c r="H7" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="43"/>
+      <c r="I7" s="46"/>
     </row>
     <row r="8" spans="2:29" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="42"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
@@ -1452,14 +1468,14 @@
       </c>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="V14" s="34" t="s">
+      <c r="V14" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="W14" s="34"/>
-      <c r="AA14" s="34" t="s">
+      <c r="W14" s="37"/>
+      <c r="AA14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="34"/>
+      <c r="AB14" s="37"/>
     </row>
     <row r="16" spans="2:29" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K16" s="19" t="s">

</xml_diff>

<commit_message>
report 2-4 for testing
</commit_message>
<xml_diff>
--- a/src/main/resources/patterns.xlsx
+++ b/src/main/resources/patterns.xlsx
@@ -616,23 +616,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1122,7 +1122,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="35" t="s">
@@ -1142,20 +1142,20 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
@@ -1350,14 +1350,14 @@
       </c>
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="V14" s="39" t="s">
+      <c r="V14" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="W14" s="39"/>
-      <c r="AA14" s="39" t="s">
+      <c r="W14" s="44"/>
+      <c r="AA14" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="AB14" s="39"/>
+      <c r="AB14" s="44"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
       <c r="C15" s="30" t="s">
@@ -1427,7 +1427,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
+      <c r="N17" s="20"/>
       <c r="O17" s="14"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>

</xml_diff>

<commit_message>
one fix five in proccess
</commit_message>
<xml_diff>
--- a/src/main/resources/patterns.xlsx
+++ b/src/main/resources/patterns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Запрос 1" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -751,6 +751,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -811,6 +812,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -856,7 +860,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1165,30 +1171,30 @@
       <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="I2" s="24"/>
       <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="35"/>
+      <c r="F3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
+      <c r="G3" s="36"/>
       <c r="I3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1221,8 +1227,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1247,32 +1253,32 @@
       <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
@@ -1318,12 +1324,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
@@ -1346,40 +1352,40 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="37" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="44"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="45"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
@@ -1408,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17:AD17"/>
     </sheetView>
   </sheetViews>
@@ -1439,58 +1445,58 @@
     </row>
     <row r="4" spans="2:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
       <c r="J4" s="11"/>
     </row>
     <row r="5" spans="2:30" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="49" t="s">
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="2:30" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51" t="s">
+      <c r="E7" s="52"/>
+      <c r="F7" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51" t="s">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="51"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="50"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
@@ -1584,14 +1590,14 @@
       </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="V14" s="47" t="s">
+      <c r="V14" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="W14" s="47"/>
-      <c r="AA14" s="47" t="s">
+      <c r="W14" s="48"/>
+      <c r="AA14" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="AB14" s="47"/>
+      <c r="AB14" s="48"/>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C15" s="29" t="s">
@@ -1664,21 +1670,21 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
-      <c r="N17" s="67"/>
+      <c r="N17" s="32"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="67"/>
-      <c r="Q17" s="67"/>
-      <c r="R17" s="67"/>
-      <c r="S17" s="67"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
-      <c r="W17" s="67"/>
-      <c r="X17" s="67"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
       <c r="Z17" s="14"/>
       <c r="AA17" s="14"/>
-      <c r="AB17" s="67"/>
-      <c r="AC17" s="67"/>
-      <c r="AD17" s="67"/>
+      <c r="AB17" s="32"/>
+      <c r="AC17" s="32"/>
+      <c r="AD17" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1703,98 +1709,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="33"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+    </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="54" t="s">
+      <c r="E3" s="57"/>
+      <c r="F3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="54" t="s">
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="55"/>
-      <c r="R3" s="62" t="s">
+      <c r="Q3" s="57"/>
+      <c r="R3" s="64" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="63"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="65"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="33" t="s">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="33" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="34"/>
-      <c r="J5" s="33" t="s">
+      <c r="I5" s="35"/>
+      <c r="J5" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="34"/>
-      <c r="L5" s="65" t="s">
+      <c r="K5" s="35"/>
+      <c r="L5" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="66"/>
-      <c r="N5" s="33" t="s">
+      <c r="M5" s="68"/>
+      <c r="N5" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="O5" s="34"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="63"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="65"/>
     </row>
     <row r="6" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="31" t="s">
         <v>59</v>
       </c>
@@ -1837,7 +1858,7 @@
       <c r="Q6" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="64"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
@@ -1856,22 +1877,23 @@
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+      <c r="R7" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="P3:Q5"/>
+  <mergeCells count="13">
     <mergeCell ref="R3:R6"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C2:P2"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="D3:E5"/>
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="J3:O4"/>
+    <mergeCell ref="P3:Q5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
report 5 fix output
</commit_message>
<xml_diff>
--- a/src/main/resources/patterns.xlsx
+++ b/src/main/resources/patterns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Запрос 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="109">
   <si>
     <t>##</t>
   </si>
@@ -1248,21 +1248,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1296,6 +1281,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1309,41 +1309,26 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1356,16 +1341,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2245,121 +2245,117 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AA7"/>
+  <dimension ref="B2:Z7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="20" max="27" width="21.28515625" customWidth="1"/>
+    <col min="20" max="26" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="40"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-    </row>
-    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="68" t="s">
+      <c r="E3" s="64"/>
+      <c r="F3" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="68" t="s">
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="68" t="s">
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="60" t="s">
+      <c r="Q3" s="64"/>
+      <c r="R3" s="71" t="s">
         <v>57</v>
       </c>
       <c r="T3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="W3" s="19" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="X3" s="19" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="Y3" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA3" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="70"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="61"/>
+    <row r="4" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="72"/>
       <c r="T4" s="14"/>
       <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="39"/>
+      <c r="V4" s="39"/>
+      <c r="W4" s="14"/>
       <c r="X4" s="14"/>
       <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="39"/>
-    </row>
-    <row r="5" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="73"/>
+      <c r="Z4" s="39"/>
+    </row>
+    <row r="5" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="41" t="s">
         <v>4</v>
       </c>
@@ -2372,21 +2368,21 @@
         <v>29</v>
       </c>
       <c r="K5" s="42"/>
-      <c r="L5" s="63" t="s">
+      <c r="L5" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="64"/>
+      <c r="M5" s="75"/>
       <c r="N5" s="41" t="s">
         <v>58</v>
       </c>
       <c r="O5" s="42"/>
-      <c r="P5" s="72"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="61"/>
-    </row>
-    <row r="6" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="72"/>
+    </row>
+    <row r="6" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="31" t="s">
         <v>59</v>
       </c>
@@ -2429,9 +2425,9 @@
       <c r="Q6" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="62"/>
-    </row>
-    <row r="7" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="73"/>
+    </row>
+    <row r="7" spans="2:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -2452,6 +2448,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R3:R6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="C2:P2"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="B3:B6"/>
@@ -2459,12 +2461,6 @@
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="J3:O4"/>
     <mergeCell ref="P3:Q5"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2590,7 +2586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2605,69 +2601,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
     </row>
     <row r="3" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="83" t="s">
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="82" t="s">
+      <c r="H3" s="92"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82" t="s">
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82" t="s">
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="S3" s="82"/>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="94" t="s">
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="94"/>
-      <c r="AA3" s="94"/>
-      <c r="AB3" s="94"/>
-      <c r="AC3" s="94"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="89"/>
       <c r="AE3" s="19" t="s">
         <v>12</v>
       </c>
@@ -2700,179 +2696,179 @@
       </c>
     </row>
     <row r="4" spans="2:40" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="82"/>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
-      <c r="AB4" s="94"/>
-      <c r="AC4" s="94"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="89"/>
       <c r="AJ4" s="37"/>
     </row>
     <row r="5" spans="2:40" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="82"/>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="94"/>
-      <c r="W5" s="94"/>
-      <c r="X5" s="94"/>
-      <c r="Y5" s="94"/>
-      <c r="Z5" s="94"/>
-      <c r="AA5" s="94"/>
-      <c r="AB5" s="94"/>
-      <c r="AC5" s="94"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
+      <c r="Z5" s="89"/>
+      <c r="AA5" s="89"/>
+      <c r="AB5" s="89"/>
+      <c r="AC5" s="89"/>
     </row>
     <row r="6" spans="2:40" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="81" t="s">
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="81" t="s">
+      <c r="I6" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="92" t="s">
+      <c r="J6" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="92" t="s">
+      <c r="K6" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="L6" s="92" t="s">
+      <c r="L6" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="M6" s="92" t="s">
+      <c r="M6" s="87" t="s">
         <v>85</v>
       </c>
-      <c r="N6" s="92" t="s">
+      <c r="N6" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="O6" s="92" t="s">
+      <c r="O6" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="P6" s="92" t="s">
+      <c r="P6" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="Q6" s="92" t="s">
+      <c r="Q6" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="92" t="s">
+      <c r="R6" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="S6" s="92" t="s">
+      <c r="S6" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="T6" s="92" t="s">
+      <c r="T6" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="U6" s="92" t="s">
+      <c r="U6" s="87" t="s">
         <v>86</v>
       </c>
-      <c r="V6" s="81" t="s">
+      <c r="V6" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="W6" s="81" t="s">
+      <c r="W6" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="X6" s="82" t="s">
+      <c r="X6" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="82" t="s">
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="AA6" s="82"/>
-      <c r="AB6" s="82"/>
-      <c r="AC6" s="82"/>
+      <c r="AA6" s="81"/>
+      <c r="AB6" s="81"/>
+      <c r="AC6" s="81"/>
     </row>
     <row r="7" spans="2:40" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="92"/>
-      <c r="O7" s="92"/>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="92"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="92"/>
-      <c r="U7" s="92"/>
-      <c r="V7" s="81"/>
-      <c r="W7" s="81"/>
-      <c r="X7" s="96" t="s">
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="86"/>
+      <c r="W7" s="86"/>
+      <c r="X7" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="Y7" s="96" t="s">
+      <c r="Y7" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="Z7" s="97" t="s">
+      <c r="Z7" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="AA7" s="98" t="s">
+      <c r="AA7" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="AB7" s="98" t="s">
+      <c r="AB7" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="AC7" s="98" t="s">
+      <c r="AC7" s="84" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:40" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="95"/>
-      <c r="C8" s="81"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="86"/>
       <c r="D8" s="36" t="s">
         <v>96</v>
       </c>
@@ -2882,29 +2878,29 @@
       <c r="F8" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="92"/>
-      <c r="R8" s="92"/>
-      <c r="S8" s="92"/>
-      <c r="T8" s="92"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="81"/>
-      <c r="W8" s="81"/>
-      <c r="X8" s="96"/>
-      <c r="Y8" s="96"/>
-      <c r="Z8" s="97"/>
-      <c r="AA8" s="98"/>
-      <c r="AB8" s="99"/>
-      <c r="AC8" s="99"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="87"/>
+      <c r="K8" s="87"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="86"/>
+      <c r="W8" s="86"/>
+      <c r="X8" s="82"/>
+      <c r="Y8" s="82"/>
+      <c r="Z8" s="83"/>
+      <c r="AA8" s="84"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="85"/>
     </row>
     <row r="9" spans="2:40" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38"/>
@@ -2938,14 +2934,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="Z6:AC6"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="Z7:Z8"/>
-    <mergeCell ref="AA7:AA8"/>
-    <mergeCell ref="AB7:AB8"/>
-    <mergeCell ref="AC7:AC8"/>
-    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:F7"/>
+    <mergeCell ref="G3:I5"/>
+    <mergeCell ref="J3:M5"/>
+    <mergeCell ref="L6:L8"/>
+    <mergeCell ref="M6:M8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="J6:J8"/>
+    <mergeCell ref="K6:K8"/>
     <mergeCell ref="W6:W8"/>
     <mergeCell ref="R6:R8"/>
     <mergeCell ref="N6:N8"/>
@@ -2962,16 +2960,14 @@
     <mergeCell ref="O6:O8"/>
     <mergeCell ref="P6:P8"/>
     <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:F7"/>
-    <mergeCell ref="G3:I5"/>
-    <mergeCell ref="J3:M5"/>
-    <mergeCell ref="L6:L8"/>
-    <mergeCell ref="M6:M8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="J6:J8"/>
-    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="X7:X8"/>
+    <mergeCell ref="Y7:Y8"/>
+    <mergeCell ref="Z7:Z8"/>
+    <mergeCell ref="AA7:AA8"/>
+    <mergeCell ref="AB7:AB8"/>
+    <mergeCell ref="AC7:AC8"/>
+    <mergeCell ref="X6:Y6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>